<commit_message>
CAN1-66 update acceptance filter testcases
added note regarding masking register testing - Devon
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/acceptance_filter_testcases.xlsx
+++ b/Documentations/Test Cases/acceptance_filter_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22274E2-EC8C-44CB-9457-BD0A9DF2AC6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6B6755-F23A-4852-BA75-B25463BB0C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
   </bookViews>
@@ -528,12 +528,6 @@
     <t>AFR4.AFMR = M</t>
   </si>
   <si>
-    <t xml:space="preserve">set 'i_afir3' to some arbitrary value, Y
-set 'i_rx_message'[127:96] equal to Y except for some bits
-set 'i_afmr3' to exclude the differing bits
-set 'i_uaf3' to 1 </t>
-  </si>
-  <si>
     <t>set 'i_afmr3' to now include the differing bits</t>
   </si>
   <si>
@@ -568,6 +562,13 @@
     <t>set uaf bits back to 0
 set i_afir and i_afmr inputs to arbitrary values
 check internal ID register in submodules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note: Mask testing one submodule covers masking register functionality for all submodules
+set 'i_afir3' to some arbitrary value, Y
+set 'i_rx_message'[127:96] equal to Y except for some bits
+set 'i_afmr3' to exclude the differing bits
+set 'i_uaf3' to 1 </t>
   </si>
 </sst>
 </file>
@@ -639,17 +640,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -659,6 +651,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -979,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73642E39-ECFF-4314-AFC1-488407319D91}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,10 +1036,10 @@
       <c r="C2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="12" t="s">
         <v>92</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1055,8 +1056,8 @@
       <c r="C3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="13"/>
       <c r="F3" s="5" t="s">
         <v>94</v>
       </c>
@@ -1091,8 +1092,8 @@
       <c r="D5" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>152</v>
+      <c r="E5" s="8" t="s">
+        <v>151</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>96</v>
@@ -1111,7 +1112,7 @@
       <c r="D6" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="8" t="s">
         <v>104</v>
       </c>
       <c r="F6" s="5" t="s">
@@ -1131,8 +1132,8 @@
       <c r="D7" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>153</v>
+      <c r="E7" s="8" t="s">
+        <v>152</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>102</v>
@@ -1151,14 +1152,14 @@
       <c r="D8" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="8" t="s">
         <v>106</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1169,10 +1170,10 @@
         <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>154</v>
+        <v>157</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>153</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>99</v>
@@ -1189,10 +1190,10 @@
         <v>75</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>155</v>
+        <v>150</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>154</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>100</v>
@@ -1211,8 +1212,8 @@
       <c r="D11" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>156</v>
+      <c r="E11" s="8" t="s">
+        <v>155</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>101</v>
@@ -1231,7 +1232,7 @@
       <c r="D12" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="8" t="s">
         <v>109</v>
       </c>
       <c r="F12" s="5" t="s">
@@ -1251,7 +1252,7 @@
       <c r="D13" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F13" s="5" t="s">
@@ -1265,13 +1266,13 @@
       <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="8" t="s">
         <v>121</v>
       </c>
       <c r="F14" s="4" t="s">
@@ -1291,7 +1292,7 @@
       <c r="D15" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="10" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1308,7 +1309,7 @@
       <c r="D16" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="8" t="s">
         <v>119</v>
       </c>
       <c r="F16" s="5" t="s">
@@ -1328,7 +1329,7 @@
       <c r="D17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>117</v>
       </c>
       <c r="F17" s="5" t="s">
@@ -1342,10 +1343,10 @@
       <c r="B18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="11" t="s">
         <v>125</v>
       </c>
       <c r="E18" s="14" t="s">
@@ -1365,7 +1366,7 @@
       <c r="C19" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="14"/>
       <c r="F19" s="5" t="s">
         <v>127</v>
@@ -1381,7 +1382,7 @@
       <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="14"/>
       <c r="F20" s="5" t="s">
         <v>128</v>
@@ -1397,10 +1398,10 @@
       <c r="C21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="10" t="s">
         <v>132</v>
       </c>
       <c r="F21" s="5" t="s">
@@ -1417,10 +1418,10 @@
       <c r="C22" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="E22" s="11" t="s">
+      <c r="D22" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>134</v>
       </c>
       <c r="F22" t="s">
@@ -1437,8 +1438,8 @@
       <c r="C23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="13" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="10" t="s">
         <v>138</v>
       </c>
       <c r="F23" t="s">
@@ -1455,8 +1456,8 @@
       <c r="C24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="13" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="10" t="s">
         <v>139</v>
       </c>
       <c r="F24" t="s">
@@ -1473,8 +1474,8 @@
       <c r="C25" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="13" t="s">
+      <c r="D25" s="11"/>
+      <c r="E25" s="10" t="s">
         <v>140</v>
       </c>
       <c r="F25" t="s">
@@ -1491,8 +1492,8 @@
       <c r="C26" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="13" t="s">
+      <c r="D26" s="11"/>
+      <c r="E26" s="10" t="s">
         <v>142</v>
       </c>
       <c r="F26" t="s">
@@ -1509,8 +1510,8 @@
       <c r="C27" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="13" t="s">
+      <c r="D27" s="11"/>
+      <c r="E27" s="10" t="s">
         <v>144</v>
       </c>
       <c r="F27" t="s">
@@ -1527,8 +1528,8 @@
       <c r="C28" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="13" t="s">
+      <c r="D28" s="11"/>
+      <c r="E28" s="10" t="s">
         <v>146</v>
       </c>
       <c r="F28" t="s">
@@ -1545,8 +1546,8 @@
       <c r="C29" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="13" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="10" t="s">
         <v>148</v>
       </c>
       <c r="F29" t="s">

</xml_diff>

<commit_message>
CAN1-66 acceptance filter testcases revision
removed irrelevant signal assignments from TC_01, added expected result to TC_14, added test step to internal register assignment tests. -Devon
</commit_message>
<xml_diff>
--- a/Documentations/Test Cases/acceptance_filter_testcases.xlsx
+++ b/Documentations/Test Cases/acceptance_filter_testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\CAN_we_do_it_Can_Controller\Documentations\Test Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6B6755-F23A-4852-BA75-B25463BB0C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A9A96C-8F91-499A-9C46-70B5F7395A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D9DD170-8ED8-4417-B493-FE566D307589}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="159">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -432,12 +432,6 @@
 set 'i_rx_full' to 0</t>
   </si>
   <si>
-    <t>Instantiate module
-set 'i_reset' to 1
-set 'i_can_ready' to 1
-set 'i_rx_full' to 0</t>
-  </si>
-  <si>
     <t>o_rx_w_en' = 1 for one system clock cycle</t>
   </si>
   <si>
@@ -559,16 +553,24 @@
 'i_afir4'[31:0] = Z</t>
   </si>
   <si>
-    <t>set uaf bits back to 0
-set i_afir and i_afmr inputs to arbitrary values
-check internal ID register in submodules</t>
-  </si>
-  <si>
     <t xml:space="preserve">Note: Mask testing one submodule covers masking register functionality for all submodules
 set 'i_afir3' to some arbitrary value, Y
 set 'i_rx_message'[127:96] equal to Y except for some bits
 set 'i_afmr3' to exclude the differing bits
 set 'i_uaf3' to 1 </t>
+  </si>
+  <si>
+    <t>Instantiate module
+set 'i_reset' to 1</t>
+  </si>
+  <si>
+    <t>currstate' = idle</t>
+  </si>
+  <si>
+    <t>set uaf bits back to 0
+set i_afir and i_afmr inputs to arbitrary values
+check internal ID register in submodules
+check internal mask register in submodules</t>
   </si>
 </sst>
 </file>
@@ -980,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73642E39-ECFF-4314-AFC1-488407319D91}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1039,7 @@
         <v>67</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>92</v>
@@ -1093,7 +1095,7 @@
         <v>111</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>96</v>
@@ -1133,7 +1135,7 @@
         <v>105</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>102</v>
@@ -1170,10 +1172,10 @@
         <v>74</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>99</v>
@@ -1190,10 +1192,10 @@
         <v>75</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>100</v>
@@ -1213,7 +1215,7 @@
         <v>108</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>101</v>
@@ -1247,7 +1249,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>122</v>
@@ -1256,7 +1258,7 @@
         <v>110</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="156" customHeight="1" x14ac:dyDescent="0.25">
@@ -1295,6 +1297,9 @@
       <c r="E15" s="10" t="s">
         <v>114</v>
       </c>
+      <c r="F15" s="5" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1347,13 +1352,13 @@
         <v>66</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="14" t="s">
-        <v>126</v>
-      </c>
       <c r="F18" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1369,7 +1374,7 @@
       <c r="D19" s="11"/>
       <c r="E19" s="14"/>
       <c r="F19" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1385,7 +1390,7 @@
       <c r="D20" s="11"/>
       <c r="E20" s="14"/>
       <c r="F20" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,13 +1404,13 @@
         <v>82</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E21" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F21" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1419,13 +1424,13 @@
         <v>83</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E22" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" t="s">
         <v>134</v>
-      </c>
-      <c r="F22" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
@@ -1440,10 +1445,10 @@
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,10 +1463,10 @@
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1476,10 +1481,10 @@
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="F25" t="s">
         <v>140</v>
-      </c>
-      <c r="F25" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1494,10 +1499,10 @@
       </c>
       <c r="D26" s="11"/>
       <c r="E26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" t="s">
         <v>142</v>
-      </c>
-      <c r="F26" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
@@ -1512,10 +1517,10 @@
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F27" t="s">
         <v>144</v>
-      </c>
-      <c r="F27" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1530,10 +1535,10 @@
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F28" t="s">
         <v>146</v>
-      </c>
-      <c r="F28" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1548,10 +1553,10 @@
       </c>
       <c r="D29" s="11"/>
       <c r="E29" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" t="s">
         <v>148</v>
-      </c>
-      <c r="F29" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>